<commit_message>
Redactada parte 1 evaluación práctica 3, añadida gráfica de tiempo de ejecución para distintos tamaños de bloque a resultados
</commit_message>
<xml_diff>
--- a/practicas/practica3/resultados.xlsx
+++ b/practicas/practica3/resultados.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="11">
   <si>
     <t>Función</t>
   </si>
@@ -53,50 +53,20 @@
     <t>Speedup</t>
   </si>
   <si>
-    <t>RGB2YCbCr_block()_2</t>
+    <t>-</t>
   </si>
   <si>
-    <t>RGB2YCbCr_block()_4</t>
+    <t>BLOCK</t>
   </si>
   <si>
-    <t>RGB2YCbCr_block()_8</t>
-  </si>
-  <si>
-    <t>RGB2YCbCr_block()_16</t>
-  </si>
-  <si>
-    <t>RGB2YCbCr_block()_32</t>
-  </si>
-  <si>
-    <t>RGB2YCbCr_block()_64</t>
-  </si>
-  <si>
-    <t>RGB2YCbCr_block()_128</t>
-  </si>
-  <si>
-    <t>RGB2YCbCr_block()_256</t>
-  </si>
-  <si>
-    <t>RGB2YCbCr_block()_512</t>
-  </si>
-  <si>
-    <t>RGB2YCbCr_block()_1024</t>
-  </si>
-  <si>
-    <t>RGB2YCbCr_block()_2048</t>
-  </si>
-  <si>
-    <t>RGB2YCbCr_block()_4096</t>
-  </si>
-  <si>
-    <t>-</t>
+    <t>RGB2YCbCr_block()</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -127,21 +97,50 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
@@ -150,9 +149,29 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Hipervínculo" xfId="1" builtinId="8" hidden="1"/>
@@ -167,6 +186,1062 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="es-ES"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="es-ES_tradnl"/>
+              <a:t>Speedup para RGB2YCbCr_block()</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="es-ES_tradnl" baseline="0"/>
+              <a:t> en función del tamaño de bloque</a:t>
+            </a:r>
+            <a:endParaRPr lang="es-ES_tradnl"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="es-ES_tradnl"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Hoja1!$B$5:$B$14</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>2.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>8.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>16.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>32.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>64.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>128.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>256.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>512.0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1024.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Hoja1!$F$5:$F$14</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>1.41304347826087</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.533018867924528</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.533018867924528</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.785714285714286</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2.044025157232704</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2.288732394366197</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2.407407407407407</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2.372262773722627</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2.407407407407407</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>2.480916030534351</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:hiLowLines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="75000"/>
+                  <a:lumOff val="25000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:hiLowLines>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="736711088"/>
+        <c:axId val="736713136"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="736711088"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="es-ES_tradnl"/>
+                  <a:t>Tamaño de bloque</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="es-ES_tradnl"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="es-ES_tradnl"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="736713136"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="736713136"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="es-ES_tradnl"/>
+                  <a:t>Speedup</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="es-ES_tradnl"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="es-ES_tradnl"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="736711088"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="es-ES_tradnl"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="332">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>426720</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>30480</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>254000</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>40640</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Gráfico 1"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -432,305 +1507,350 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E16"/>
+  <dimension ref="A1:F16"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="22.33203125" customWidth="1"/>
+    <col min="1" max="1" width="18.6640625" style="2" customWidth="1"/>
+    <col min="2" max="2" width="9.83203125" style="1" customWidth="1"/>
+    <col min="3" max="6" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" s="6" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A2" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B2">
+      <c r="B2" s="4"/>
+      <c r="C2" s="4">
         <v>3.25</v>
       </c>
-      <c r="C2">
+      <c r="D2" s="4">
         <v>6.5</v>
       </c>
-      <c r="D2">
+      <c r="E2" s="4">
         <v>0.15</v>
       </c>
-      <c r="E2">
-        <f>$B$2/B2</f>
+      <c r="F2" s="4">
+        <f>$C$2/C2</f>
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A3" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B3">
+      <c r="B3" s="4"/>
+      <c r="C3" s="4">
         <v>2.17</v>
       </c>
-      <c r="C3">
+      <c r="D3" s="4">
         <v>4.3</v>
       </c>
-      <c r="D3">
+      <c r="E3" s="4">
         <v>0.23</v>
       </c>
-      <c r="E3">
-        <f t="shared" ref="E3:E16" si="0">$B$2/B3</f>
+      <c r="F3" s="4">
+        <f t="shared" ref="F3:F16" si="0">$C$2/C3</f>
         <v>1.4976958525345623</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A4" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B4">
+      <c r="B4" s="4"/>
+      <c r="C4" s="4">
         <v>0.5</v>
       </c>
-      <c r="C4">
+      <c r="D4" s="4">
         <v>1</v>
       </c>
-      <c r="D4">
+      <c r="E4" s="4">
         <v>1.01</v>
       </c>
-      <c r="E4">
+      <c r="F4" s="4">
         <f t="shared" si="0"/>
         <v>6.5</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>8</v>
-      </c>
-      <c r="B5">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A5" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5" s="4">
+        <v>2</v>
+      </c>
+      <c r="C5" s="4">
         <v>2.2999999999999998</v>
       </c>
-      <c r="C5">
+      <c r="D5" s="4">
         <v>4.5999999999999996</v>
       </c>
-      <c r="D5">
+      <c r="E5" s="4">
         <v>0.22</v>
       </c>
-      <c r="E5">
+      <c r="F5" s="4">
         <f t="shared" si="0"/>
         <v>1.4130434782608696</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
-        <v>9</v>
-      </c>
-      <c r="B6">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A6" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6" s="4">
+        <v>4</v>
+      </c>
+      <c r="C6" s="4">
         <v>2.12</v>
       </c>
-      <c r="C6">
+      <c r="D6" s="4">
         <v>4.2</v>
       </c>
-      <c r="D6">
+      <c r="E6" s="4">
         <v>0.24</v>
       </c>
-      <c r="E6">
+      <c r="F6" s="4">
         <f t="shared" si="0"/>
         <v>1.5330188679245282</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A7" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="B7">
+      <c r="B7" s="4">
+        <v>8</v>
+      </c>
+      <c r="C7" s="4">
         <v>2.12</v>
       </c>
-      <c r="C7">
+      <c r="D7" s="4">
         <v>4.2</v>
       </c>
-      <c r="D7">
+      <c r="E7" s="4">
         <v>0.24</v>
       </c>
-      <c r="E7">
+      <c r="F7" s="4">
         <f t="shared" si="0"/>
         <v>1.5330188679245282</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
-        <v>11</v>
-      </c>
-      <c r="B8">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A8" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B8" s="4">
+        <v>16</v>
+      </c>
+      <c r="C8" s="4">
         <v>1.82</v>
       </c>
-      <c r="C8">
+      <c r="D8" s="4">
         <v>3.6</v>
       </c>
-      <c r="D8">
+      <c r="E8" s="4">
         <v>0.28000000000000003</v>
       </c>
-      <c r="E8">
+      <c r="F8" s="4">
         <f t="shared" si="0"/>
         <v>1.7857142857142856</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
-        <v>12</v>
-      </c>
-      <c r="B9">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A9" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B9" s="4">
+        <v>32</v>
+      </c>
+      <c r="C9" s="4">
         <v>1.59</v>
       </c>
-      <c r="C9">
+      <c r="D9" s="4">
         <v>3.2</v>
       </c>
-      <c r="D9">
+      <c r="E9" s="4">
         <v>0.32</v>
       </c>
-      <c r="E9">
+      <c r="F9" s="4">
         <f t="shared" si="0"/>
         <v>2.0440251572327042</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
-        <v>13</v>
-      </c>
-      <c r="B10">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A10" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B10" s="4">
+        <v>64</v>
+      </c>
+      <c r="C10" s="4">
         <v>1.42</v>
       </c>
-      <c r="C10">
+      <c r="D10" s="4">
         <v>2.8</v>
       </c>
-      <c r="D10">
+      <c r="E10" s="4">
         <v>0.35</v>
       </c>
-      <c r="E10">
+      <c r="F10" s="4">
         <f t="shared" si="0"/>
         <v>2.2887323943661975</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A11" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="B11">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A11" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B11" s="7">
+        <v>128</v>
+      </c>
+      <c r="C11" s="4">
         <v>1.35</v>
       </c>
-      <c r="C11">
+      <c r="D11" s="4">
         <v>2.7</v>
       </c>
-      <c r="D11">
+      <c r="E11" s="4">
         <v>0.37</v>
       </c>
-      <c r="E11">
+      <c r="F11" s="4">
         <f t="shared" si="0"/>
         <v>2.4074074074074074</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A12" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="B12">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A12" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B12" s="7">
+        <v>256</v>
+      </c>
+      <c r="C12" s="4">
         <v>1.37</v>
       </c>
-      <c r="C12">
+      <c r="D12" s="4">
         <v>2.7</v>
       </c>
-      <c r="D12">
+      <c r="E12" s="4">
         <v>0.37</v>
       </c>
-      <c r="E12">
+      <c r="F12" s="4">
         <f t="shared" si="0"/>
         <v>2.3722627737226274</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A13" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="B13">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A13" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B13" s="7">
+        <v>512</v>
+      </c>
+      <c r="C13" s="4">
         <v>1.35</v>
       </c>
-      <c r="C13">
+      <c r="D13" s="4">
         <v>2.7</v>
       </c>
-      <c r="D13">
+      <c r="E13" s="4">
         <v>0.37</v>
       </c>
-      <c r="E13">
+      <c r="F13" s="4">
         <f t="shared" si="0"/>
         <v>2.4074074074074074</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A14" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="B14">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A14" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B14" s="7">
+        <v>1024</v>
+      </c>
+      <c r="C14" s="4">
         <v>1.31</v>
       </c>
-      <c r="C14">
+      <c r="D14" s="4">
         <v>2.6</v>
       </c>
-      <c r="D14">
+      <c r="E14" s="4">
         <v>0.38</v>
       </c>
-      <c r="E14">
+      <c r="F14" s="4">
         <f t="shared" si="0"/>
         <v>2.4809160305343512</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A15" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="B15" t="s">
-        <v>20</v>
-      </c>
-      <c r="C15" t="s">
-        <v>20</v>
-      </c>
-      <c r="D15" t="s">
-        <v>20</v>
-      </c>
-      <c r="E15" t="e">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A15" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B15" s="7">
+        <v>2048</v>
+      </c>
+      <c r="C15" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D15" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="E15" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="F15" s="4" t="e">
         <f t="shared" si="0"/>
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A16" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="B16" t="s">
-        <v>20</v>
-      </c>
-      <c r="C16" t="s">
-        <v>20</v>
-      </c>
-      <c r="D16" t="s">
-        <v>20</v>
-      </c>
-      <c r="E16" t="e">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A16" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B16" s="7">
+        <v>4096</v>
+      </c>
+      <c r="C16" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D16" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="E16" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="F16" s="4" t="e">
         <f t="shared" si="0"/>
         <v>#VALUE!</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Finalizada parte obligatoria de la evaluación de la práctica 3
</commit_message>
<xml_diff>
--- a/practicas/practica3/resultados.xlsx
+++ b/practicas/practica3/resultados.xlsx
@@ -66,7 +66,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -101,6 +101,12 @@
       <b/>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -400,11 +406,11 @@
         </c:hiLowLines>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="736711088"/>
-        <c:axId val="736713136"/>
+        <c:axId val="758585344"/>
+        <c:axId val="737595392"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="736711088"/>
+        <c:axId val="758585344"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -503,7 +509,7 @@
             <a:endParaRPr lang="es-ES_tradnl"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="736713136"/>
+        <c:crossAx val="737595392"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -511,7 +517,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="736713136"/>
+        <c:axId val="737595392"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -617,7 +623,7 @@
             <a:endParaRPr lang="es-ES_tradnl"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="736711088"/>
+        <c:crossAx val="758585344"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -666,7 +672,709 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="es-ES"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="es-ES_tradnl"/>
+              <a:t>Rendimiento de las funciones</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="es-ES_tradnl"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>Speedup</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>(Hoja1!$A$2:$A$4,Hoja1!$A$14)</c:f>
+              <c:strCache>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>RGB2YCbCr_v1()</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>RGB2YCbCr_v2()</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>RGB2YCbCrSOA1()</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>RGB2YCbCr_block()</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>(Hoja1!$F$2:$F$4,Hoja1!$F$14)</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.497695852534562</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>6.5</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2.480916030534351</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="755463856"/>
+        <c:axId val="755466176"/>
+      </c:lineChart>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>Tiempo de ejecución</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>(Hoja1!$A$2:$A$4,Hoja1!$A$14)</c:f>
+              <c:strCache>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>RGB2YCbCr_v1()</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>RGB2YCbCr_v2()</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>RGB2YCbCrSOA1()</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>RGB2YCbCr_block()</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>(Hoja1!$C$2:$C$4,Hoja1!$C$14)</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>3.25</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.17</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.31</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="761098736"/>
+        <c:axId val="755097232"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="755463856"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="es-ES_tradnl"/>
+                  <a:t>Función</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="es-ES_tradnl"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="es-ES_tradnl"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="755466176"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="755466176"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="es-ES_tradnl"/>
+                  <a:t>Speedup</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="es-ES_tradnl"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="es-ES_tradnl"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="755463856"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="755097232"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="r"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="es-ES_tradnl"/>
+                  <a:t>Tiempo (segundos)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="es-ES_tradnl"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="es-ES_tradnl"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="761098736"/>
+        <c:crosses val="max"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:catAx>
+        <c:axId val="761098736"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="1"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="755097232"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="t"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="es-ES_tradnl"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="es-ES_tradnl"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
   <a:schemeClr val="accent2"/>
@@ -1209,20 +1917,523 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="332">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>426720</xdr:colOff>
+      <xdr:colOff>589280</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>30480</xdr:rowOff>
+      <xdr:rowOff>172720</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>14</xdr:col>
-      <xdr:colOff>254000</xdr:colOff>
+      <xdr:colOff>416560</xdr:colOff>
       <xdr:row>21</xdr:row>
-      <xdr:rowOff>40640</xdr:rowOff>
+      <xdr:rowOff>182880</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1236,6 +2447,36 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>203200</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>50800</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>487680</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>46000</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Gráfico 2"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -1510,7 +2751,7 @@
   <dimension ref="A1:F16"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+      <selection activeCell="L26" sqref="L26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1850,7 +3091,9 @@
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="5" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
   <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>